<commit_message>
Discretionary Data Whitelist case
Discretionary Data Whitelist case
</commit_message>
<xml_diff>
--- a/Custom_Quick Chip Mode_TW/0_Tool+doc/QuickChip test list.xlsx
+++ b/Custom_Quick Chip Mode_TW/0_Tool+doc/QuickChip test list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vivotech\regress\regression\regress_test\test_tree\Custom_Quick Chip Mode_TW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vivotech\regress\regression\regress_test\test_tree\Custom_Quick Chip Mode_TW\0_Tool+doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B86745-1F3E-467F-B7F7-5786E8E1CB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463C9791-70B0-4054-B4A2-C1F5F44F6A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="885" windowWidth="16380" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="16455" windowHeight="13455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="159">
   <si>
     <t>Item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3829,6 +3829,14 @@
 1: Start beep after sending resopnse</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Tag DFEC4F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QCM046</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -3837,7 +3845,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4041,7 +4049,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4150,9 +4158,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4185,9 +4190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4225,9 +4230,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4260,26 +4265,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4312,26 +4300,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4505,14 +4476,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.625" style="19" bestFit="1" customWidth="1"/>
@@ -4522,7 +4493,7 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4536,7 +4507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="63">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -4550,7 +4521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="127.5">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4564,7 +4535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
         <v>30</v>
       </c>
@@ -4578,7 +4549,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="63.75">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -4592,7 +4563,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="111.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="111.75">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -4609,7 +4580,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="33">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -4623,7 +4594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16.5">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -4637,7 +4608,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="78.75">
       <c r="A9" s="26" t="s">
         <v>100</v>
       </c>
@@ -4651,7 +4622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="63">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -4665,7 +4636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
@@ -4679,7 +4650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -4693,7 +4664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="31.5">
       <c r="A13" s="23" t="s">
         <v>65</v>
       </c>
@@ -4707,8 +4678,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:5" ht="31.5">
+      <c r="A14" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -4721,8 +4692,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
+    <row r="15" spans="1:5" ht="31.5">
+      <c r="A15" s="37"/>
       <c r="B15" s="32" t="s">
         <v>135</v>
       </c>
@@ -4733,8 +4704,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+    <row r="16" spans="1:5" ht="31.5">
+      <c r="A16" s="38"/>
       <c r="B16" s="32" t="s">
         <v>128</v>
       </c>
@@ -4745,8 +4716,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+    <row r="17" spans="1:4" ht="31.5">
+      <c r="A17" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -4759,8 +4730,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+    <row r="18" spans="1:4" ht="31.5">
+      <c r="A18" s="37"/>
       <c r="B18" s="32" t="s">
         <v>130</v>
       </c>
@@ -4771,8 +4742,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+    <row r="19" spans="1:4" ht="31.5">
+      <c r="A19" s="38"/>
       <c r="B19" s="32" t="s">
         <v>131</v>
       </c>
@@ -4781,8 +4752,8 @@
       </c>
       <c r="D19" s="34"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="32" t="s">
@@ -4795,8 +4766,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
+    <row r="21" spans="1:4">
+      <c r="A21" s="37"/>
       <c r="B21" s="32" t="s">
         <v>132</v>
       </c>
@@ -4807,8 +4778,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
+    <row r="22" spans="1:4">
+      <c r="A22" s="37"/>
       <c r="B22" s="32" t="s">
         <v>124</v>
       </c>
@@ -4817,8 +4788,8 @@
       </c>
       <c r="D22" s="34"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+    <row r="23" spans="1:4">
+      <c r="A23" s="38"/>
       <c r="B23" s="32" t="s">
         <v>127</v>
       </c>
@@ -4829,7 +4800,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16.5">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -4843,7 +4814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16.5">
       <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
@@ -4857,7 +4828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="31.5">
       <c r="A26" s="2" t="s">
         <v>67</v>
       </c>
@@ -4871,7 +4842,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="31.5">
       <c r="A27" s="2" t="s">
         <v>69</v>
       </c>
@@ -4885,7 +4856,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
@@ -4899,7 +4870,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16.5">
       <c r="A29" s="31" t="s">
         <v>5</v>
       </c>
@@ -4913,7 +4884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16.5">
       <c r="A30" s="31" t="s">
         <v>5</v>
       </c>
@@ -4927,7 +4898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16.5">
       <c r="A31" s="6" t="s">
         <v>89</v>
       </c>
@@ -4941,7 +4912,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16.5">
       <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
@@ -4955,7 +4926,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16.5">
       <c r="A33" s="7" t="s">
         <v>88</v>
       </c>
@@ -4969,7 +4940,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="16.5">
       <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
@@ -4983,7 +4954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="63">
       <c r="A35" s="6" t="s">
         <v>5</v>
       </c>
@@ -4997,7 +4968,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="31.5">
       <c r="A36" s="6" t="s">
         <v>5</v>
       </c>
@@ -5011,7 +4982,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="6" t="s">
         <v>5</v>
       </c>
@@ -5023,11 +4994,11 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="7" t="s">
         <v>146</v>
       </c>
       <c r="C38" s="25" t="s">
@@ -5037,7 +5008,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="6" t="s">
         <v>5</v>
       </c>
@@ -5049,7 +5020,7 @@
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="31" t="s">
         <v>5</v>
       </c>
@@ -5063,7 +5034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="6" t="s">
         <v>5</v>
       </c>
@@ -5077,7 +5048,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="6" t="s">
         <v>5</v>
       </c>
@@ -5091,7 +5062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="6" t="s">
         <v>5</v>
       </c>
@@ -5105,7 +5076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="6" t="s">
         <v>5</v>
       </c>
@@ -5119,7 +5090,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="6" t="s">
         <v>5</v>
       </c>
@@ -5133,7 +5104,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="6" t="s">
         <v>5</v>
       </c>
@@ -5147,7 +5118,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="31.5">
       <c r="A47" s="6" t="s">
         <v>5</v>
       </c>
@@ -5161,7 +5132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="31.5">
       <c r="A48" s="2" t="s">
         <v>152</v>
       </c>
@@ -5175,7 +5146,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="47.25">
       <c r="A49" s="6" t="s">
         <v>5</v>
       </c>
@@ -5186,6 +5157,18 @@
         <v>155</v>
       </c>
       <c r="D49" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2"/>
+      <c r="B50" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5210,7 +5193,7 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.25" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="66.875" style="12" customWidth="1"/>
@@ -5218,7 +5201,7 @@
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -5232,7 +5215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="69.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5246,7 +5229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="69.75" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -5258,7 +5241,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="69" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -5272,7 +5255,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="35.25" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -5286,7 +5269,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="213.75" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -5314,7 +5297,7 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="24.5" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="61.875" style="12" customWidth="1"/>
@@ -5322,7 +5305,7 @@
     <col min="5" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -5336,7 +5319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="252" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="252">
       <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
@@ -5350,7 +5333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="236.25">
       <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
@@ -5380,7 +5363,7 @@
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="17.25" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.5" style="12" customWidth="1"/>
@@ -5389,7 +5372,7 @@
     <col min="5" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -5403,7 +5386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="337.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="337.5" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -5417,7 +5400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="260.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="260.25" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -5431,7 +5414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="299.25">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -5445,7 +5428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="362.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="362.25" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -5459,7 +5442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="330.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="330.75">
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
@@ -5473,7 +5456,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="378" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="378">
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>

</xml_diff>